<commit_message>
Fixed some of the test names.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>(SBAC_PT)SBAC-IRP-CAT-MATH-3-Summer-2015-2016</t>
   </si>
   <si>
-    <t>(SBAC_PT)SBAC-IRP-Perf-MATH-3-Summer-2015-2018</t>
-  </si>
-  <si>
     <t>(SBAC_PT)IRP-Perf-ELA-7-Summer-2015-2016</t>
   </si>
   <si>
@@ -63,10 +60,13 @@
     <t>(SBAC_PT)SBAC-IRP-CAT-MATH-11-Summer-2015-2016</t>
   </si>
   <si>
-    <t>(SBAC_PT)SBAC-IRP-Perf-MATH-11-Summer-2015-2018</t>
-  </si>
-  <si>
     <t>Directions: Register each of the following students (Column B) with the corresponding test (Column A)</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-MATH-3-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-MATH-11-Summer-2015-2016</t>
   </si>
 </sst>
 </file>
@@ -123,8 +123,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="145">
+  <cellStyleXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -277,7 +279,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="145">
+  <cellStyles count="147">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -350,6 +352,7 @@
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -422,6 +425,7 @@
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -792,13 +796,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -884,7 +888,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>39990010</v>
@@ -892,7 +896,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>39990011</v>
@@ -900,7 +904,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>39990012</v>
@@ -908,7 +912,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>79990001</v>
@@ -916,7 +920,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>79990002</v>
@@ -924,7 +928,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>79990003</v>
@@ -932,7 +936,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>79990004</v>
@@ -940,7 +944,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>79990005</v>
@@ -948,7 +952,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20">
         <v>79990006</v>
@@ -956,7 +960,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>79990007</v>
@@ -964,7 +968,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22">
         <v>79990008</v>
@@ -972,7 +976,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>79990009</v>
@@ -980,7 +984,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>79990010</v>
@@ -988,7 +992,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>79990011</v>
@@ -996,7 +1000,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26">
         <v>79990012</v>
@@ -1004,7 +1008,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>119990001</v>
@@ -1012,7 +1016,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>119990002</v>
@@ -1020,7 +1024,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>119990003</v>
@@ -1028,7 +1032,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>119990004</v>
@@ -1036,7 +1040,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>119990005</v>
@@ -1044,7 +1048,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>119990006</v>
@@ -1052,7 +1056,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33">
         <v>119990007</v>
@@ -1060,7 +1064,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34">
         <v>119990008</v>
@@ -1068,7 +1072,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <v>119990009</v>
@@ -1076,7 +1080,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B36">
         <v>119990010</v>
@@ -1084,7 +1088,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B37">
         <v>119990011</v>
@@ -1092,7 +1096,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B38">
         <v>119990012</v>

</xml_diff>

<commit_message>
Added Alternate SSID and Student Name to the Test-Student Mapping Excel file so it’s easier for vendors to get the information they need without having to cross reference between two files.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t>Test</t>
   </si>
@@ -67,13 +67,235 @@
   </si>
   <si>
     <t>(SBAC_PT)SBAC-IRP-Perf-MATH-11-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>StudentA</t>
+  </si>
+  <si>
+    <t>StudentB</t>
+  </si>
+  <si>
+    <t>StudentC</t>
+  </si>
+  <si>
+    <t>StudentD</t>
+  </si>
+  <si>
+    <t>StudentE</t>
+  </si>
+  <si>
+    <t>StudentF</t>
+  </si>
+  <si>
+    <t>StudentG</t>
+  </si>
+  <si>
+    <t>StudentH</t>
+  </si>
+  <si>
+    <t>StudentI</t>
+  </si>
+  <si>
+    <t>StudentJ</t>
+  </si>
+  <si>
+    <t>StudentK</t>
+  </si>
+  <si>
+    <t>StudentL</t>
+  </si>
+  <si>
+    <t>StudentM</t>
+  </si>
+  <si>
+    <t>StudentN</t>
+  </si>
+  <si>
+    <t>StudentO</t>
+  </si>
+  <si>
+    <t>StudentP</t>
+  </si>
+  <si>
+    <t>StudentQ</t>
+  </si>
+  <si>
+    <t>StudentR</t>
+  </si>
+  <si>
+    <t>StudentS</t>
+  </si>
+  <si>
+    <t>StudentT</t>
+  </si>
+  <si>
+    <t>StudentU</t>
+  </si>
+  <si>
+    <t>StudentV</t>
+  </si>
+  <si>
+    <t>StudentW</t>
+  </si>
+  <si>
+    <t>StudentX</t>
+  </si>
+  <si>
+    <t>StudentY</t>
+  </si>
+  <si>
+    <t>StudentZ</t>
+  </si>
+  <si>
+    <t>StudentAA</t>
+  </si>
+  <si>
+    <t>StudentAB</t>
+  </si>
+  <si>
+    <t>StudentAC</t>
+  </si>
+  <si>
+    <t>StudentAD</t>
+  </si>
+  <si>
+    <t>StudentAE</t>
+  </si>
+  <si>
+    <t>StudentAF</t>
+  </si>
+  <si>
+    <t>StudentAG</t>
+  </si>
+  <si>
+    <t>StudentAH</t>
+  </si>
+  <si>
+    <t>StudentAI</t>
+  </si>
+  <si>
+    <t>StudentAJ</t>
+  </si>
+  <si>
+    <t>AlternateSSID</t>
+  </si>
+  <si>
+    <t>A39990001</t>
+  </si>
+  <si>
+    <t>A39990002</t>
+  </si>
+  <si>
+    <t>A39990003</t>
+  </si>
+  <si>
+    <t>A39990004</t>
+  </si>
+  <si>
+    <t>A39990005</t>
+  </si>
+  <si>
+    <t>A39990006</t>
+  </si>
+  <si>
+    <t>A39990007</t>
+  </si>
+  <si>
+    <t>A39990008</t>
+  </si>
+  <si>
+    <t>A39990009</t>
+  </si>
+  <si>
+    <t>A39990010</t>
+  </si>
+  <si>
+    <t>A39990011</t>
+  </si>
+  <si>
+    <t>A39990012</t>
+  </si>
+  <si>
+    <t>A79990001</t>
+  </si>
+  <si>
+    <t>A79990002</t>
+  </si>
+  <si>
+    <t>A79990003</t>
+  </si>
+  <si>
+    <t>A79990004</t>
+  </si>
+  <si>
+    <t>A79990005</t>
+  </si>
+  <si>
+    <t>A79990006</t>
+  </si>
+  <si>
+    <t>A79990007</t>
+  </si>
+  <si>
+    <t>A79990008</t>
+  </si>
+  <si>
+    <t>A79990009</t>
+  </si>
+  <si>
+    <t>A79990010</t>
+  </si>
+  <si>
+    <t>A79990011</t>
+  </si>
+  <si>
+    <t>A79990012</t>
+  </si>
+  <si>
+    <t>A119990001</t>
+  </si>
+  <si>
+    <t>A119990002</t>
+  </si>
+  <si>
+    <t>A119990003</t>
+  </si>
+  <si>
+    <t>A119990004</t>
+  </si>
+  <si>
+    <t>A119990005</t>
+  </si>
+  <si>
+    <t>A119990006</t>
+  </si>
+  <si>
+    <t>A119990007</t>
+  </si>
+  <si>
+    <t>A119990008</t>
+  </si>
+  <si>
+    <t>A119990009</t>
+  </si>
+  <si>
+    <t>A119990010</t>
+  </si>
+  <si>
+    <t>A119990011</t>
+  </si>
+  <si>
+    <t>A119990012</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,6 +327,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -272,11 +498,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="147">
@@ -788,318 +1019,544 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="30" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>39990001</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>39990002</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
         <v>39990003</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>39990004</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <v>39990005</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>39990006</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9">
         <v>39990007</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10">
         <v>39990008</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11">
         <v>39990009</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>39990010</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>39990011</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>39990012</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15">
         <v>79990001</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16">
         <v>79990002</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17">
         <v>79990003</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18">
         <v>79990004</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19">
         <v>79990005</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20">
         <v>79990006</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21">
         <v>79990007</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22">
         <v>79990008</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23">
         <v>79990009</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24">
         <v>79990010</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25">
         <v>79990011</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="B26">
         <v>79990012</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>9</v>
       </c>
       <c r="B27">
         <v>119990001</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28">
         <v>119990002</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29">
         <v>119990003</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>10</v>
       </c>
       <c r="B30">
         <v>119990004</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>10</v>
       </c>
       <c r="B31">
         <v>119990005</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>10</v>
       </c>
       <c r="B32">
         <v>119990006</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33">
         <v>119990007</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>11</v>
       </c>
       <c r="B34">
         <v>119990008</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>11</v>
       </c>
       <c r="B35">
         <v>119990009</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>14</v>
       </c>
       <c r="B36">
         <v>119990010</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>14</v>
       </c>
       <c r="B37">
         <v>119990011</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>14</v>
       </c>
       <c r="B38">
         <v>119990012</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1108,7 +1565,7 @@
     <sortCondition ref="A3:A38"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
updating to handle CAT style test packages.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="90">
   <si>
     <t>Test</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>A119990012</t>
+  </si>
+  <si>
+    <t>CAT</t>
   </si>
 </sst>
 </file>
@@ -1019,543 +1022,592 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="47.375" customWidth="1"/>
+    <col min="2" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>39990001</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>39990002</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
         <v>39990003</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>39990004</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <v>39990005</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>39990006</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9">
         <v>39990007</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10">
         <v>39990008</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11">
         <v>39990009</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>39990010</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>39990011</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>39990012</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15">
         <v>79990001</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16">
         <v>79990002</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17">
         <v>79990003</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18">
         <v>79990004</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19">
         <v>79990005</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20">
         <v>79990006</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21">
         <v>79990007</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22">
         <v>79990008</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23">
         <v>79990009</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24">
         <v>79990010</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25">
         <v>79990011</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="B26">
         <v>79990012</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
       <c r="B27">
         <v>119990001</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28">
         <v>119990002</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29">
         <v>119990003</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
       <c r="B30">
         <v>119990004</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
       <c r="B31">
         <v>119990005</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
       <c r="B32">
         <v>119990006</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33">
         <v>119990007</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
       <c r="B34">
         <v>119990008</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
       <c r="B35">
         <v>119990009</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
       <c r="B36">
         <v>119990010</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
       <c r="B37">
         <v>119990011</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
       <c r="B38">
         <v>119990012</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1565,7 +1617,7 @@
     <sortCondition ref="A3:A38"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
As dates are stored as numbers in Excel (IRPStudents .xlsx), modified to convert to Java date
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -1025,7 +1025,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1050,10 +1050,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>52</v>
@@ -1066,7 +1066,7 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>39990001</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1080,7 +1080,7 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>39990002</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1094,7 +1094,7 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>39990003</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1108,11 +1108,11 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>39990004</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>56</v>
@@ -1125,11 +1125,11 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>39990005</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>57</v>
@@ -1142,11 +1142,11 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>39990006</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>58</v>
@@ -1159,11 +1159,11 @@
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>39990007</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>59</v>
@@ -1176,11 +1176,11 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10">
         <v>39990008</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>60</v>
@@ -1193,11 +1193,11 @@
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>39990009</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>61</v>
@@ -1210,7 +1210,7 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>39990010</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1224,7 +1224,7 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>39990011</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1238,7 +1238,7 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>39990012</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1252,7 +1252,7 @@
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>79990001</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1266,7 +1266,7 @@
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>79990002</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1280,7 +1280,7 @@
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>79990003</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1294,11 +1294,11 @@
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18">
         <v>79990004</v>
-      </c>
-      <c r="C18" t="b">
-        <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>68</v>
@@ -1311,11 +1311,11 @@
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>79990005</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>69</v>
@@ -1328,11 +1328,11 @@
       <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>79990006</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>70</v>
@@ -1345,7 +1345,7 @@
       <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>79990007</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1359,7 +1359,7 @@
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>79990008</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1373,7 +1373,7 @@
       <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>79990009</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -1387,7 +1387,7 @@
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>79990010</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -1401,7 +1401,7 @@
       <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>79990011</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -1415,7 +1415,7 @@
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>79990012</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -1429,7 +1429,7 @@
       <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>119990001</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -1443,7 +1443,7 @@
       <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>119990002</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -1457,7 +1457,7 @@
       <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>119990003</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -1471,11 +1471,11 @@
       <c r="A30" t="s">
         <v>10</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30">
         <v>119990004</v>
-      </c>
-      <c r="C30" t="b">
-        <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>80</v>
@@ -1488,11 +1488,11 @@
       <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31">
         <v>119990005</v>
-      </c>
-      <c r="C31" t="b">
-        <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>81</v>
@@ -1505,11 +1505,11 @@
       <c r="A32" t="s">
         <v>10</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32">
         <v>119990006</v>
-      </c>
-      <c r="C32" t="b">
-        <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>82</v>
@@ -1522,11 +1522,11 @@
       <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33">
         <v>119990007</v>
-      </c>
-      <c r="C33" t="b">
-        <v>1</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>83</v>
@@ -1539,11 +1539,11 @@
       <c r="A34" t="s">
         <v>11</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34">
         <v>119990008</v>
-      </c>
-      <c r="C34" t="b">
-        <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>84</v>
@@ -1556,11 +1556,11 @@
       <c r="A35" t="s">
         <v>11</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35">
         <v>119990009</v>
-      </c>
-      <c r="C35" t="b">
-        <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>85</v>
@@ -1573,7 +1573,7 @@
       <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>119990010</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -1587,7 +1587,7 @@
       <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>119990011</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -1601,7 +1601,7 @@
       <c r="A38" t="s">
         <v>14</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>119990012</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -1613,7 +1613,6 @@
     </row>
   </sheetData>
   <sortState ref="A3:B38">
-    <sortCondition ref="B3:B38"/>
     <sortCondition ref="A3:A38"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>

<commit_message>
regarding combined test packages revised TestStudentMapping file added related Combined test packages files modified code to handle revised TestStudentMapping objects Combined and Individual test packages can be parse accordingly.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="40380" windowHeight="25995" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="OLE_LINK7" localSheetId="0">Sheet1!$A$41</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="108">
   <si>
     <t>Test</t>
   </si>
@@ -292,6 +293,60 @@
   </si>
   <si>
     <t>CAT</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-ELA-7-COMBINED-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-MATH-3-COMBINED-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-CAT-COMBINED-ELA-7-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-S1-COMBINED-ELA-7-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-S2-COMBINED-ELA-7-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-CAT-COMBINED-MATH-3-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-COMBINED-MATH-3-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>StudentAK</t>
+  </si>
+  <si>
+    <t>StudentAL</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-ELA-3-COMBINED-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-ELA-11-COMBINED-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-MATH-7-COMBINED-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-MATH-11-COMBINED-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>please add</t>
   </si>
 </sst>
 </file>
@@ -352,7 +407,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="147">
+  <cellStyleXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -500,8 +555,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -509,11 +580,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="147">
+  <cellStyles count="163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -587,6 +659,14 @@
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -660,6 +740,14 @@
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1022,593 +1110,1085 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.375" customWidth="1"/>
-    <col min="2" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" customWidth="1"/>
+    <col min="3" max="3" width="62.5" customWidth="1"/>
+    <col min="4" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="13.125" customWidth="1"/>
+    <col min="7" max="7" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>39990001</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>39990002</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>39990003</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="b">
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="b">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>39990004</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="b">
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="b">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>39990005</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="b">
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="b">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>39990006</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="b">
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="b">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>39990007</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="b">
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="b">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>39990008</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="b">
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="b">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>39990009</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12">
         <v>39990010</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13">
         <v>39990011</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14">
         <v>39990012</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="C15">
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
         <v>79990001</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="C16">
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
         <v>79990002</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="C17">
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
         <v>79990003</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" t="b">
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="b">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>79990004</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" t="b">
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="b">
         <v>1</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>79990005</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B20" t="b">
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="b">
         <v>1</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>79990006</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="C21">
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21">
         <v>79990007</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="C22">
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22">
         <v>79990008</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="C23">
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23">
         <v>79990009</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="C24">
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24">
         <v>79990010</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="C25">
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25">
         <v>79990011</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="C26">
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26">
         <v>79990012</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="C27">
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27">
         <v>119990001</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="C28">
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28">
         <v>119990002</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="C29">
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29">
         <v>119990003</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
-      <c r="B30" t="b">
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="b">
         <v>1</v>
       </c>
-      <c r="C30">
+      <c r="E30">
         <v>119990004</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="B31" t="b">
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="b">
         <v>1</v>
       </c>
-      <c r="C31">
+      <c r="E31">
         <v>119990005</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
-      <c r="B32" t="b">
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="b">
         <v>1</v>
       </c>
-      <c r="C32">
+      <c r="E32">
         <v>119990006</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B33" t="b">
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="b">
         <v>1</v>
       </c>
-      <c r="C33">
+      <c r="E33">
         <v>119990007</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
-      <c r="B34" t="b">
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="b">
         <v>1</v>
       </c>
-      <c r="C34">
+      <c r="E34">
         <v>119990008</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
-      <c r="B35" t="b">
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="b">
         <v>1</v>
       </c>
-      <c r="C35">
+      <c r="E35">
         <v>119990009</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="C36">
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36">
         <v>119990010</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="C37">
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37">
         <v>119990011</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C38">
+      <c r="B38" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38">
         <v>119990012</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>79990001</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42">
+        <v>79990001</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43">
+        <v>79990001</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" t="s">
+        <v>107</v>
+      </c>
+      <c r="F44" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>39990007</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47">
+        <v>39990007</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F49" t="s">
+        <v>107</v>
+      </c>
+      <c r="G49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" t="s">
+        <v>107</v>
+      </c>
+      <c r="F50" t="s">
+        <v>107</v>
+      </c>
+      <c r="G50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" t="s">
+        <v>107</v>
+      </c>
+      <c r="G51" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1616,14 +2196,9 @@
     <sortCondition ref="A3:A38"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
revised IRPTestStudentMapping.xlsx and updated related code
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="OLE_LINK7" localSheetId="0">Sheet1!$A$41</definedName>
+    <definedName name="OLE_LINK7" localSheetId="0">Sheet1!$A$42</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="120">
   <si>
     <t>Test</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Single</t>
   </si>
   <si>
-    <t>Segment</t>
-  </si>
-  <si>
     <t>(SBAC_PT)SBAC-IRP-ELA-7-COMBINED-Summer-2015-2016</t>
   </si>
   <si>
@@ -347,6 +344,45 @@
   </si>
   <si>
     <t>please add</t>
+  </si>
+  <si>
+    <t>ComponentTestName</t>
+  </si>
+  <si>
+    <t>SegmentName</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-S1-COMBINED-ELA-3-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-S2-COMBINED-ELA-3-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-CAT-COMBINED-ELA-3-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-S1-COMBINED-ELA-11-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-S2-COMBINED-ELA-11-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-CAT-COMBINED-ELA-11-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-COMBINED-MATH-7-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-CAT-Calc-COMBINED-MATH-7-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-CAT-NoCalc-COMBINED-MATH-7-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-Perf-COMBINED-MATH-11-Summer-2015-2016</t>
+  </si>
+  <si>
+    <t>(SBAC_PT)SBAC-IRP-CAT-COMBINED-MATH-11-Summer-2015-2016</t>
   </si>
 </sst>
 </file>
@@ -1110,23 +1146,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="3" width="62.5" customWidth="1"/>
-    <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
-    <col min="7" max="7" width="12.875" customWidth="1"/>
+    <col min="3" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1136,8 +1172,9 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1145,22 +1182,25 @@
         <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1170,17 +1210,20 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>39990001</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1190,17 +1233,20 @@
       <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>39990002</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1210,17 +1256,20 @@
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>39990003</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1230,20 +1279,23 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6">
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>39990004</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1253,20 +1305,23 @@
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7">
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>39990005</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1276,20 +1331,23 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>39990006</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1299,20 +1357,23 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>39990007</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1322,20 +1383,23 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>39990008</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1345,20 +1409,23 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11">
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>39990009</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1368,17 +1435,20 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="E12">
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12">
         <v>39990010</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1388,17 +1458,20 @@
       <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="E13">
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13">
         <v>39990011</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1408,17 +1481,20 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="E14">
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14">
         <v>39990012</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1428,17 +1504,20 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="E15">
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15">
         <v>79990001</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1448,17 +1527,20 @@
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="E16">
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16">
         <v>79990002</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1468,17 +1550,20 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-      <c r="E17">
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17">
         <v>79990003</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1488,20 +1573,23 @@
       <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18">
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>79990004</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1511,20 +1599,23 @@
       <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19">
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>79990005</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1534,20 +1625,23 @@
       <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20">
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>79990006</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1557,17 +1651,20 @@
       <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="E21">
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21">
         <v>79990007</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1577,17 +1674,20 @@
       <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="E22">
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22">
         <v>79990008</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1597,17 +1697,20 @@
       <c r="C23" t="s">
         <v>7</v>
       </c>
-      <c r="E23">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23">
         <v>79990009</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1617,17 +1720,20 @@
       <c r="C24" t="s">
         <v>8</v>
       </c>
-      <c r="E24">
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
         <v>79990010</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1637,17 +1743,20 @@
       <c r="C25" t="s">
         <v>8</v>
       </c>
-      <c r="E25">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25">
         <v>79990011</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1657,17 +1766,20 @@
       <c r="C26" t="s">
         <v>8</v>
       </c>
-      <c r="E26">
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26">
         <v>79990012</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1677,17 +1789,20 @@
       <c r="C27" t="s">
         <v>9</v>
       </c>
-      <c r="E27">
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27">
         <v>119990001</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1697,17 +1812,20 @@
       <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="E28">
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28">
         <v>119990002</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1717,17 +1835,20 @@
       <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="E29">
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29">
         <v>119990003</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1737,20 +1858,23 @@
       <c r="C30" t="s">
         <v>10</v>
       </c>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30">
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30">
         <v>119990004</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1760,20 +1884,23 @@
       <c r="C31" t="s">
         <v>10</v>
       </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31">
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>119990005</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1783,20 +1910,23 @@
       <c r="C32" t="s">
         <v>10</v>
       </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32">
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32">
         <v>119990006</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1806,20 +1936,23 @@
       <c r="C33" t="s">
         <v>11</v>
       </c>
-      <c r="D33" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33">
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>119990007</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1829,20 +1962,23 @@
       <c r="C34" t="s">
         <v>11</v>
       </c>
-      <c r="D34" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34">
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <v>119990008</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1852,20 +1988,23 @@
       <c r="C35" t="s">
         <v>11</v>
       </c>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35">
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <v>119990009</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1875,17 +2014,20 @@
       <c r="C36" t="s">
         <v>14</v>
       </c>
-      <c r="E36">
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36">
         <v>119990010</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1895,17 +2037,20 @@
       <c r="C37" t="s">
         <v>14</v>
       </c>
-      <c r="E37">
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37">
         <v>119990011</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>14</v>
       </c>
@@ -1915,280 +2060,406 @@
       <c r="C38" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E38">
+      <c r="D38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38">
         <v>119990012</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E39" t="s">
-        <v>107</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>94</v>
+        <v>110</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>102</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>79990001</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E42">
+        <v>96</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42">
         <v>79990001</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E43">
+        <v>97</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43">
         <v>79990001</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C44" t="s">
-        <v>107</v>
-      </c>
-      <c r="E44" t="s">
-        <v>107</v>
-      </c>
-      <c r="F44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>79990001</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
         <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
-      </c>
-      <c r="E45" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
       </c>
       <c r="F45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G45" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="H45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B46" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>39990007</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" s="5" t="s">
+      <c r="C46" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" t="s">
+        <v>106</v>
+      </c>
+      <c r="H46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E47">
-        <v>39990007</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>106</v>
+      </c>
+      <c r="G47" t="s">
+        <v>106</v>
+      </c>
+      <c r="H47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C48" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48" t="s">
-        <v>107</v>
-      </c>
-      <c r="F48" t="s">
-        <v>107</v>
-      </c>
-      <c r="G48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48">
+        <v>39990007</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C49" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" t="s">
-        <v>107</v>
-      </c>
-      <c r="F49" t="s">
-        <v>107</v>
-      </c>
-      <c r="G49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>39990007</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
-      </c>
-      <c r="E50" t="s">
-        <v>107</v>
+        <v>115</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G50" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="H50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>107</v>
-      </c>
-      <c r="E51" t="s">
-        <v>107</v>
+        <v>116</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G51" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="H51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>106</v>
+      </c>
+      <c r="G52" t="s">
+        <v>106</v>
+      </c>
+      <c r="H52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
+        <v>106</v>
+      </c>
+      <c r="G53" t="s">
+        <v>106</v>
+      </c>
+      <c r="H53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>106</v>
+      </c>
+      <c r="G54" t="s">
+        <v>106</v>
+      </c>
+      <c r="H54" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2196,7 +2467,7 @@
     <sortCondition ref="A3:A38"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added students to student mapping
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPTestStudentMapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="40380" windowHeight="25995" tabRatio="500"/>
+    <workbookView xWindow="8800" yWindow="1780" windowWidth="29520" windowHeight="20160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="119">
   <si>
     <t>Test</t>
   </si>
@@ -341,9 +341,6 @@
   </si>
   <si>
     <t>(SBAC_PT)SBAC-IRP-MATH-11-COMBINED-Summer-2015-2016</t>
-  </si>
-  <si>
-    <t>please add</t>
   </si>
   <si>
     <t>ComponentTestName</t>
@@ -389,7 +386,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -425,6 +422,20 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -443,7 +454,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -607,8 +618,70 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -620,8 +693,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -703,6 +778,38 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -784,6 +891,36 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1146,23 +1283,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="4" width="62.5" customWidth="1"/>
     <col min="5" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
-    <col min="8" max="8" width="12.875" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="32" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="14" width="21.1640625" customWidth="1"/>
+    <col min="15" max="15" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1174,7 +1317,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1182,10 +1325,10 @@
         <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>89</v>
@@ -1200,7 +1343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1223,7 +1366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1246,7 +1389,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1269,7 +1412,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1295,7 +1438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1321,7 +1464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1347,7 +1490,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1516,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1399,7 +1542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1448,7 +1591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1471,7 +1614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1494,7 +1637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1517,7 +1660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1540,7 +1683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1563,7 +1706,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1589,7 +1732,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1615,7 +1758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1641,7 +1784,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1664,7 +1807,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1687,7 +1830,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1710,7 +1853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1733,7 +1876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1756,7 +1899,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1778,8 +1921,9 @@
       <c r="H26" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M26" s="7"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1801,8 +1945,9 @@
       <c r="H27" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1824,8 +1969,9 @@
       <c r="H28" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1847,8 +1993,9 @@
       <c r="H29" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1874,7 +2021,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1900,7 +2047,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1926,7 +2073,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1952,7 +2099,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1978,7 +2125,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2004,7 +2151,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2027,7 +2174,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2050,7 +2197,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="5" t="s">
         <v>14</v>
       </c>
@@ -2073,7 +2220,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="5" t="s">
         <v>102</v>
       </c>
@@ -2081,22 +2228,22 @@
         <v>91</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F39" t="s">
-        <v>106</v>
+      <c r="F39">
+        <v>39990001</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="5" t="s">
         <v>102</v>
       </c>
@@ -2104,22 +2251,22 @@
         <v>91</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F40" t="s">
-        <v>106</v>
+      <c r="F40">
+        <v>39990001</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2127,7 +2274,7 @@
         <v>91</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>3</v>
@@ -2135,17 +2282,17 @@
       <c r="E41" t="b">
         <v>1</v>
       </c>
-      <c r="F41" t="s">
-        <v>106</v>
+      <c r="F41">
+        <v>39990001</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="5" t="s">
         <v>93</v>
       </c>
@@ -2168,7 +2315,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="5" t="s">
         <v>93</v>
       </c>
@@ -2191,7 +2338,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="5" t="s">
         <v>93</v>
       </c>
@@ -2217,7 +2364,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="5" t="s">
         <v>103</v>
       </c>
@@ -2225,22 +2372,22 @@
         <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
       </c>
-      <c r="F45" t="s">
-        <v>106</v>
-      </c>
-      <c r="G45" t="s">
-        <v>106</v>
-      </c>
-      <c r="H45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>119990001</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="5" t="s">
         <v>103</v>
       </c>
@@ -2248,22 +2395,22 @@
         <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
       </c>
-      <c r="F46" t="s">
-        <v>106</v>
-      </c>
-      <c r="G46" t="s">
-        <v>106</v>
-      </c>
-      <c r="H46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>119990001</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -2271,7 +2418,7 @@
         <v>91</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
         <v>10</v>
@@ -2279,17 +2426,17 @@
       <c r="E47" t="b">
         <v>1</v>
       </c>
-      <c r="F47" t="s">
-        <v>106</v>
-      </c>
-      <c r="G47" t="s">
-        <v>106</v>
-      </c>
-      <c r="H47" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>119990001</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="5" t="s">
         <v>94</v>
       </c>
@@ -2312,7 +2459,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="5" t="s">
         <v>94</v>
       </c>
@@ -2338,7 +2485,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="5" t="s">
         <v>104</v>
       </c>
@@ -2346,22 +2493,22 @@
         <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
       </c>
-      <c r="F50" t="s">
-        <v>106</v>
-      </c>
-      <c r="G50" t="s">
-        <v>106</v>
-      </c>
-      <c r="H50" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>79990007</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="5" t="s">
         <v>104</v>
       </c>
@@ -2369,7 +2516,7 @@
         <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -2377,17 +2524,17 @@
       <c r="E51" t="b">
         <v>1</v>
       </c>
-      <c r="F51" t="s">
-        <v>106</v>
-      </c>
-      <c r="G51" t="s">
-        <v>106</v>
-      </c>
-      <c r="H51" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>79990007</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -2395,7 +2542,7 @@
         <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -2403,17 +2550,17 @@
       <c r="E52" t="b">
         <v>1</v>
       </c>
-      <c r="F52" t="s">
-        <v>106</v>
-      </c>
-      <c r="G52" t="s">
-        <v>106</v>
-      </c>
-      <c r="H52" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>79990007</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="5" t="s">
         <v>105</v>
       </c>
@@ -2421,22 +2568,22 @@
         <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D53" t="s">
         <v>14</v>
       </c>
-      <c r="F53" t="s">
-        <v>106</v>
-      </c>
-      <c r="G53" t="s">
-        <v>106</v>
-      </c>
-      <c r="H53" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>119990007</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="5" t="s">
         <v>105</v>
       </c>
@@ -2444,7 +2591,7 @@
         <v>91</v>
       </c>
       <c r="C54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -2452,14 +2599,14 @@
       <c r="E54" t="b">
         <v>1</v>
       </c>
-      <c r="F54" t="s">
-        <v>106</v>
-      </c>
-      <c r="G54" t="s">
-        <v>106</v>
-      </c>
-      <c r="H54" t="s">
-        <v>106</v>
+      <c r="F54">
+        <v>119990007</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2471,5 +2618,10 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>